<commit_message>
Tippfehler und Nummerierung der Reihenfolge
</commit_message>
<xml_diff>
--- a/Beispiel2_Service_Value_Chain.xlsx
+++ b/Beispiel2_Service_Value_Chain.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t xml:space="preserve">Service Chain Activity</t>
   </si>
@@ -35,6 +35,36 @@
   </si>
   <si>
     <t xml:space="preserve">Praktiken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informations-Sicherheit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wissensmanagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Messen und Dokumentieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risikomanagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zulieferermanagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incidentmanagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT-Kapitalmanagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problemmanagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Releasemanagement</t>
   </si>
 </sst>
 </file>
@@ -49,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -70,6 +101,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -126,28 +158,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,58 +276,171 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="2" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="0"/>
-      <c r="O1" s="0"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Beispiel2 (Austaus eines Mitarbeiter-Laptops) aktualisiert
</commit_message>
<xml_diff>
--- a/Beispiel2_Service_Value_Chain.xlsx
+++ b/Beispiel2_Service_Value_Chain.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t xml:space="preserve">Service Chain Activity</t>
   </si>
@@ -28,10 +28,10 @@
     <t xml:space="preserve">Einbringen</t>
   </si>
   <si>
-    <t xml:space="preserve">Erhalten / Entwickeln</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausliefern / Supporten</t>
+    <t xml:space="preserve">Erhalten/ Entwickeln</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausliefern &amp; Supporten</t>
   </si>
   <si>
     <t xml:space="preserve">Praktiken</t>
@@ -183,16 +183,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -278,17 +278,17 @@
   </sheetPr>
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="2" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -301,18 +301,20 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="7"/>
+      <c r="N1" s="0"/>
+      <c r="O1" s="0"/>
+      <c r="P1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -321,18 +323,11 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="E2" s="4"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -347,6 +342,9 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E3" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
@@ -361,6 +359,9 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E4" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -375,17 +376,24 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E5" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -397,61 +405,38 @@
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E11" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="8">
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>

</xml_diff>

<commit_message>
Beispiel: "Austausch Mitarbeiterlaptop" erweitert.
</commit_message>
<xml_diff>
--- a/Beispiel2_Service_Value_Chain.xlsx
+++ b/Beispiel2_Service_Value_Chain.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="19">
   <si>
     <t xml:space="preserve">Service Chain Activity</t>
   </si>
@@ -61,10 +61,22 @@
     <t xml:space="preserve">IT-Kapitalmanagement</t>
   </si>
   <si>
+    <t xml:space="preserve">IT-Assetmanagement</t>
+  </si>
+  <si>
     <t xml:space="preserve">Problemmanagement</t>
   </si>
   <si>
+    <t xml:space="preserve">(X)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Releasemanagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deploymentmanagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servicevalidierungs- &amp; ~test</t>
   </si>
 </sst>
 </file>
@@ -276,16 +288,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="2" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.68"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -411,25 +424,73 @@
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E9" s="8"/>
+      <c r="F9" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>